<commit_message>
mysql is optimized for inquire
</commit_message>
<xml_diff>
--- a/CheckData.xlsx
+++ b/CheckData.xlsx
@@ -2544,7 +2544,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -2935,7 +2935,7 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -2982,7 +2982,7 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -3029,7 +3029,7 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -3326,7 +3326,7 @@
         <v>0</v>
       </c>
       <c r="J18">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K18">
         <v>0</v>
@@ -3373,7 +3373,7 @@
         <v>0</v>
       </c>
       <c r="J19">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K19">
         <v>0</v>
@@ -3420,7 +3420,7 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K20">
         <v>0</v>
@@ -3517,7 +3517,7 @@
         <v>0</v>
       </c>
       <c r="J22">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K22">
         <v>0</v>
@@ -3564,7 +3564,7 @@
         <v>0</v>
       </c>
       <c r="J23">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K23">
         <v>0</v>
@@ -3661,7 +3661,7 @@
         <v>0</v>
       </c>
       <c r="J25">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K25">
         <v>0</v>
@@ -3708,7 +3708,7 @@
         <v>0</v>
       </c>
       <c r="J26">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K26">
         <v>0</v>
@@ -3805,7 +3805,7 @@
         <v>0</v>
       </c>
       <c r="J28">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K28">
         <v>0</v>
@@ -3852,7 +3852,7 @@
         <v>0</v>
       </c>
       <c r="J29">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K29">
         <v>0</v>
@@ -4099,7 +4099,7 @@
         <v>0</v>
       </c>
       <c r="J34">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K34">
         <v>0</v>
@@ -4396,7 +4396,7 @@
         <v>0</v>
       </c>
       <c r="J40">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K40">
         <v>0</v>
@@ -4443,7 +4443,7 @@
         <v>0</v>
       </c>
       <c r="J41">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K41">
         <v>0</v>
@@ -4490,7 +4490,7 @@
         <v>0</v>
       </c>
       <c r="J42">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K42">
         <v>0</v>
@@ -4587,7 +4587,7 @@
         <v>0</v>
       </c>
       <c r="J44">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K44">
         <v>0</v>
@@ -4634,7 +4634,7 @@
         <v>0</v>
       </c>
       <c r="J45">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K45">
         <v>0</v>
@@ -4681,7 +4681,7 @@
         <v>0</v>
       </c>
       <c r="J46">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K46">
         <v>0</v>
@@ -4728,7 +4728,7 @@
         <v>0</v>
       </c>
       <c r="J47">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K47">
         <v>0</v>
@@ -4775,7 +4775,7 @@
         <v>0</v>
       </c>
       <c r="J48">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K48">
         <v>0</v>
@@ -4822,7 +4822,7 @@
         <v>0</v>
       </c>
       <c r="J49">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K49">
         <v>0</v>
@@ -4969,7 +4969,7 @@
         <v>0</v>
       </c>
       <c r="J52">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K52">
         <v>0</v>
@@ -5016,7 +5016,7 @@
         <v>0</v>
       </c>
       <c r="J53">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K53">
         <v>0</v>
@@ -5063,7 +5063,7 @@
         <v>0</v>
       </c>
       <c r="J54">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K54">
         <v>0</v>
@@ -5110,7 +5110,7 @@
         <v>0</v>
       </c>
       <c r="J55">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K55">
         <v>0</v>
@@ -5257,7 +5257,7 @@
         <v>0</v>
       </c>
       <c r="J58">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K58">
         <v>0</v>
@@ -5454,7 +5454,7 @@
         <v>0</v>
       </c>
       <c r="J62">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K62">
         <v>0</v>
@@ -5501,7 +5501,7 @@
         <v>0</v>
       </c>
       <c r="J63">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K63">
         <v>0</v>
@@ -5548,7 +5548,7 @@
         <v>0</v>
       </c>
       <c r="J64">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K64">
         <v>0</v>
@@ -5595,7 +5595,7 @@
         <v>0</v>
       </c>
       <c r="J65">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K65">
         <v>0</v>
@@ -5642,7 +5642,7 @@
         <v>0</v>
       </c>
       <c r="J66">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K66">
         <v>0</v>
@@ -5689,7 +5689,7 @@
         <v>0</v>
       </c>
       <c r="J67">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K67">
         <v>0</v>
@@ -5736,7 +5736,7 @@
         <v>0</v>
       </c>
       <c r="J68">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K68">
         <v>0</v>
@@ -5783,7 +5783,7 @@
         <v>0</v>
       </c>
       <c r="J69">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K69">
         <v>0</v>
@@ -5830,7 +5830,7 @@
         <v>0</v>
       </c>
       <c r="J70">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K70">
         <v>0</v>
@@ -5877,7 +5877,7 @@
         <v>0</v>
       </c>
       <c r="J71">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K71">
         <v>0</v>
@@ -6074,7 +6074,7 @@
         <v>0</v>
       </c>
       <c r="J75">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K75">
         <v>0</v>
@@ -6121,7 +6121,7 @@
         <v>0</v>
       </c>
       <c r="J76">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K76">
         <v>0</v>
@@ -6168,7 +6168,7 @@
         <v>0</v>
       </c>
       <c r="J77">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K77">
         <v>0</v>
@@ -6215,7 +6215,7 @@
         <v>0</v>
       </c>
       <c r="J78">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K78">
         <v>0</v>
@@ -6306,7 +6306,7 @@
         <v>0</v>
       </c>
       <c r="J80">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K80">
         <v>0</v>
@@ -6353,7 +6353,7 @@
         <v>0</v>
       </c>
       <c r="J81">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K81">
         <v>0</v>
@@ -6400,7 +6400,7 @@
         <v>0</v>
       </c>
       <c r="J82">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K82">
         <v>0</v>
@@ -6447,7 +6447,7 @@
         <v>0</v>
       </c>
       <c r="J83">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K83">
         <v>0</v>
@@ -6494,7 +6494,7 @@
         <v>0</v>
       </c>
       <c r="J84">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K84">
         <v>0</v>
@@ -6541,7 +6541,7 @@
         <v>0</v>
       </c>
       <c r="J85">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K85">
         <v>0</v>
@@ -6688,7 +6688,7 @@
         <v>0</v>
       </c>
       <c r="J88">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K88">
         <v>0</v>
@@ -6785,7 +6785,7 @@
         <v>0</v>
       </c>
       <c r="J90">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K90">
         <v>0</v>
@@ -6832,7 +6832,7 @@
         <v>0</v>
       </c>
       <c r="J91">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K91">
         <v>0</v>
@@ -6879,7 +6879,7 @@
         <v>0</v>
       </c>
       <c r="J92">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K92">
         <v>0</v>
@@ -6926,7 +6926,7 @@
         <v>0</v>
       </c>
       <c r="J93">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K93">
         <v>0</v>
@@ -6973,7 +6973,7 @@
         <v>0</v>
       </c>
       <c r="J94">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K94">
         <v>0</v>
@@ -7020,7 +7020,7 @@
         <v>0</v>
       </c>
       <c r="J95">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K95">
         <v>0</v>
@@ -7067,7 +7067,7 @@
         <v>0</v>
       </c>
       <c r="J96">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K96">
         <v>0</v>
@@ -7214,7 +7214,7 @@
         <v>0</v>
       </c>
       <c r="J99">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K99">
         <v>0</v>
@@ -7261,7 +7261,7 @@
         <v>0</v>
       </c>
       <c r="J100">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K100">
         <v>0</v>
@@ -7308,7 +7308,7 @@
         <v>0</v>
       </c>
       <c r="J101">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K101">
         <v>0</v>
@@ -7405,7 +7405,7 @@
         <v>0</v>
       </c>
       <c r="J103">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K103">
         <v>0</v>
@@ -7452,7 +7452,7 @@
         <v>0</v>
       </c>
       <c r="J104">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K104">
         <v>0</v>
@@ -7499,7 +7499,7 @@
         <v>0</v>
       </c>
       <c r="J105">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K105">
         <v>0</v>
@@ -7596,7 +7596,7 @@
         <v>0</v>
       </c>
       <c r="J107">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K107">
         <v>0</v>
@@ -7693,7 +7693,7 @@
         <v>0</v>
       </c>
       <c r="J109">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K109">
         <v>0</v>
@@ -7940,7 +7940,7 @@
         <v>0</v>
       </c>
       <c r="J114">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K114">
         <v>0</v>
@@ -8187,7 +8187,7 @@
         <v>0</v>
       </c>
       <c r="J119">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K119">
         <v>0</v>
@@ -8384,7 +8384,7 @@
         <v>0</v>
       </c>
       <c r="J123">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K123">
         <v>0</v>
@@ -8431,7 +8431,7 @@
         <v>0</v>
       </c>
       <c r="J124">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K124">
         <v>0</v>
@@ -8728,7 +8728,7 @@
         <v>0</v>
       </c>
       <c r="J130">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K130">
         <v>0</v>
@@ -8775,7 +8775,7 @@
         <v>0</v>
       </c>
       <c r="J131">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K131">
         <v>0</v>
@@ -8822,7 +8822,7 @@
         <v>0</v>
       </c>
       <c r="J132">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K132">
         <v>0</v>
@@ -8869,7 +8869,7 @@
         <v>0</v>
       </c>
       <c r="J133">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K133">
         <v>0</v>
@@ -9060,7 +9060,7 @@
         <v>0</v>
       </c>
       <c r="J137">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K137">
         <v>0</v>
@@ -9107,7 +9107,7 @@
         <v>0</v>
       </c>
       <c r="J138">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K138">
         <v>0</v>
@@ -9154,7 +9154,7 @@
         <v>0</v>
       </c>
       <c r="J139">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K139">
         <v>0</v>
@@ -9201,7 +9201,7 @@
         <v>0</v>
       </c>
       <c r="J140">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K140">
         <v>0</v>
@@ -9248,7 +9248,7 @@
         <v>0</v>
       </c>
       <c r="J141">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K141">
         <v>0</v>
@@ -9295,7 +9295,7 @@
         <v>0</v>
       </c>
       <c r="J142">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K142">
         <v>0</v>
@@ -9392,7 +9392,7 @@
         <v>0</v>
       </c>
       <c r="J144">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K144">
         <v>0</v>
@@ -9439,7 +9439,7 @@
         <v>0</v>
       </c>
       <c r="J145">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K145">
         <v>0</v>
@@ -9486,7 +9486,7 @@
         <v>0</v>
       </c>
       <c r="J146">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K146">
         <v>0</v>
@@ -9533,7 +9533,7 @@
         <v>0</v>
       </c>
       <c r="J147">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K147">
         <v>0</v>
@@ -9580,7 +9580,7 @@
         <v>0</v>
       </c>
       <c r="J148">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K148">
         <v>0</v>
@@ -9671,7 +9671,7 @@
         <v>0</v>
       </c>
       <c r="J150">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K150">
         <v>0</v>
@@ -9768,7 +9768,7 @@
         <v>0</v>
       </c>
       <c r="J152">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K152">
         <v>0</v>
@@ -9815,7 +9815,7 @@
         <v>0</v>
       </c>
       <c r="J153">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K153">
         <v>0</v>
@@ -10000,7 +10000,7 @@
         <v>0</v>
       </c>
       <c r="J157">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K157">
         <v>0</v>
@@ -10047,7 +10047,7 @@
         <v>0</v>
       </c>
       <c r="J158">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K158">
         <v>0</v>
@@ -10094,7 +10094,7 @@
         <v>0</v>
       </c>
       <c r="J159">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K159">
         <v>0</v>
@@ -10835,7 +10835,7 @@
         <v>0</v>
       </c>
       <c r="J174">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K174">
         <v>0</v>
@@ -10932,7 +10932,7 @@
         <v>0</v>
       </c>
       <c r="J176">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K176">
         <v>0</v>
@@ -10979,7 +10979,7 @@
         <v>0</v>
       </c>
       <c r="J177">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K177">
         <v>0</v>
@@ -11026,7 +11026,7 @@
         <v>0</v>
       </c>
       <c r="J178">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K178">
         <v>0</v>
@@ -11117,7 +11117,7 @@
         <v>0</v>
       </c>
       <c r="J180">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K180">
         <v>0</v>
@@ -11164,7 +11164,7 @@
         <v>0</v>
       </c>
       <c r="J181">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K181">
         <v>0</v>
@@ -11211,7 +11211,7 @@
         <v>0</v>
       </c>
       <c r="J182">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K182">
         <v>0</v>
@@ -11558,7 +11558,7 @@
         <v>0</v>
       </c>
       <c r="J189">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K189">
         <v>0</v>
@@ -11743,7 +11743,7 @@
         <v>0</v>
       </c>
       <c r="J193">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K193">
         <v>0</v>
@@ -11840,7 +11840,7 @@
         <v>0</v>
       </c>
       <c r="J195">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K195">
         <v>0</v>
@@ -11937,7 +11937,7 @@
         <v>0</v>
       </c>
       <c r="J197">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K197">
         <v>0</v>
@@ -12084,7 +12084,7 @@
         <v>0</v>
       </c>
       <c r="J200">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K200">
         <v>0</v>
@@ -12131,7 +12131,7 @@
         <v>0</v>
       </c>
       <c r="J201">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K201">
         <v>0</v>
@@ -12178,7 +12178,7 @@
         <v>0</v>
       </c>
       <c r="J202">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K202">
         <v>0</v>
@@ -12275,7 +12275,7 @@
         <v>0</v>
       </c>
       <c r="J204">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K204">
         <v>0</v>
@@ -12372,7 +12372,7 @@
         <v>0</v>
       </c>
       <c r="J206">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K206">
         <v>0</v>
@@ -12519,7 +12519,7 @@
         <v>0</v>
       </c>
       <c r="J209">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K209">
         <v>0</v>
@@ -12566,7 +12566,7 @@
         <v>0</v>
       </c>
       <c r="J210">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K210">
         <v>0</v>
@@ -12713,7 +12713,7 @@
         <v>0</v>
       </c>
       <c r="J213">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K213">
         <v>0</v>
@@ -12760,7 +12760,7 @@
         <v>0</v>
       </c>
       <c r="J214">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K214">
         <v>0</v>
@@ -12895,7 +12895,7 @@
         <v>0</v>
       </c>
       <c r="J217">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K217">
         <v>0</v>
@@ -12942,7 +12942,7 @@
         <v>0</v>
       </c>
       <c r="J218">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K218">
         <v>0</v>
@@ -13221,7 +13221,7 @@
         <v>0</v>
       </c>
       <c r="J224">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K224">
         <v>0</v>
@@ -13268,7 +13268,7 @@
         <v>0</v>
       </c>
       <c r="J225">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K225">
         <v>0</v>
@@ -13315,7 +13315,7 @@
         <v>0</v>
       </c>
       <c r="J226">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K226">
         <v>0</v>
@@ -13362,7 +13362,7 @@
         <v>0</v>
       </c>
       <c r="J227">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K227">
         <v>0</v>
@@ -13553,7 +13553,7 @@
         <v>0</v>
       </c>
       <c r="J231">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K231">
         <v>0</v>
@@ -13600,7 +13600,7 @@
         <v>0</v>
       </c>
       <c r="J232">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K232">
         <v>0</v>
@@ -13647,7 +13647,7 @@
         <v>0</v>
       </c>
       <c r="J233">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K233">
         <v>0</v>
@@ -13694,7 +13694,7 @@
         <v>0</v>
       </c>
       <c r="J234">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K234">
         <v>0</v>
@@ -13741,7 +13741,7 @@
         <v>0</v>
       </c>
       <c r="J235">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K235">
         <v>0</v>
@@ -13788,7 +13788,7 @@
         <v>0</v>
       </c>
       <c r="J236">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K236">
         <v>0</v>
@@ -13835,7 +13835,7 @@
         <v>0</v>
       </c>
       <c r="J237">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K237">
         <v>0</v>
@@ -13882,7 +13882,7 @@
         <v>0</v>
       </c>
       <c r="J238">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K238">
         <v>0</v>
@@ -13973,7 +13973,7 @@
         <v>0</v>
       </c>
       <c r="J240">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K240">
         <v>0</v>
@@ -14020,7 +14020,7 @@
         <v>0</v>
       </c>
       <c r="J241">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K241">
         <v>0</v>
@@ -14067,7 +14067,7 @@
         <v>0</v>
       </c>
       <c r="J242">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K242">
         <v>0</v>
@@ -14114,7 +14114,7 @@
         <v>0</v>
       </c>
       <c r="J243">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K243">
         <v>0</v>
@@ -14161,7 +14161,7 @@
         <v>0</v>
       </c>
       <c r="J244">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K244">
         <v>0</v>
@@ -14208,7 +14208,7 @@
         <v>0</v>
       </c>
       <c r="J245">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K245">
         <v>0</v>
@@ -14299,7 +14299,7 @@
         <v>0</v>
       </c>
       <c r="J247">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K247">
         <v>0</v>
@@ -14346,7 +14346,7 @@
         <v>0</v>
       </c>
       <c r="J248">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K248">
         <v>0</v>
@@ -14393,7 +14393,7 @@
         <v>0</v>
       </c>
       <c r="J249">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K249">
         <v>0</v>
@@ -14440,7 +14440,7 @@
         <v>0</v>
       </c>
       <c r="J250">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K250">
         <v>0</v>
@@ -14487,7 +14487,7 @@
         <v>0</v>
       </c>
       <c r="J251">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K251">
         <v>0</v>
@@ -14534,7 +14534,7 @@
         <v>0</v>
       </c>
       <c r="J252">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K252">
         <v>0</v>
@@ -14581,7 +14581,7 @@
         <v>0</v>
       </c>
       <c r="J253">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K253">
         <v>0</v>
@@ -14628,7 +14628,7 @@
         <v>0</v>
       </c>
       <c r="J254">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K254">
         <v>0</v>
@@ -14675,7 +14675,7 @@
         <v>0</v>
       </c>
       <c r="J255">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K255">
         <v>0</v>
@@ -14722,7 +14722,7 @@
         <v>0</v>
       </c>
       <c r="J256">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K256">
         <v>0</v>
@@ -14769,7 +14769,7 @@
         <v>0</v>
       </c>
       <c r="J257">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K257">
         <v>0</v>
@@ -14816,7 +14816,7 @@
         <v>0</v>
       </c>
       <c r="J258">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K258">
         <v>0</v>
@@ -14863,7 +14863,7 @@
         <v>0</v>
       </c>
       <c r="J259">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K259">
         <v>0</v>
@@ -14910,7 +14910,7 @@
         <v>0</v>
       </c>
       <c r="J260">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K260">
         <v>0</v>
@@ -14957,7 +14957,7 @@
         <v>0</v>
       </c>
       <c r="J261">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K261">
         <v>0</v>
@@ -15004,7 +15004,7 @@
         <v>0</v>
       </c>
       <c r="J262">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K262">
         <v>0</v>
@@ -15051,7 +15051,7 @@
         <v>0</v>
       </c>
       <c r="J263">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K263">
         <v>0</v>
@@ -15098,7 +15098,7 @@
         <v>0</v>
       </c>
       <c r="J264">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K264">
         <v>0</v>
@@ -15145,7 +15145,7 @@
         <v>0</v>
       </c>
       <c r="J265">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K265">
         <v>0</v>
@@ -15192,7 +15192,7 @@
         <v>0</v>
       </c>
       <c r="J266">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K266">
         <v>0</v>
@@ -15239,7 +15239,7 @@
         <v>0</v>
       </c>
       <c r="J267">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K267">
         <v>0</v>
@@ -15286,7 +15286,7 @@
         <v>0</v>
       </c>
       <c r="J268">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K268">
         <v>0</v>
@@ -15377,7 +15377,7 @@
         <v>0</v>
       </c>
       <c r="J270">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K270">
         <v>0</v>
@@ -15424,7 +15424,7 @@
         <v>0</v>
       </c>
       <c r="J271">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K271">
         <v>0</v>
@@ -15471,7 +15471,7 @@
         <v>0</v>
       </c>
       <c r="J272">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K272">
         <v>0</v>
@@ -15518,7 +15518,7 @@
         <v>0</v>
       </c>
       <c r="J273">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K273">
         <v>0</v>
@@ -15565,7 +15565,7 @@
         <v>0</v>
       </c>
       <c r="J274">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K274">
         <v>0</v>
@@ -15612,7 +15612,7 @@
         <v>0</v>
       </c>
       <c r="J275">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K275">
         <v>0</v>
@@ -15659,7 +15659,7 @@
         <v>0</v>
       </c>
       <c r="J276">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K276">
         <v>0</v>
@@ -15706,7 +15706,7 @@
         <v>0</v>
       </c>
       <c r="J277">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K277">
         <v>0</v>
@@ -15797,7 +15797,7 @@
         <v>0</v>
       </c>
       <c r="J279">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K279">
         <v>0</v>
@@ -15844,7 +15844,7 @@
         <v>0</v>
       </c>
       <c r="J280">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K280">
         <v>0</v>
@@ -15891,7 +15891,7 @@
         <v>0</v>
       </c>
       <c r="J281">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K281">
         <v>0</v>
@@ -15938,7 +15938,7 @@
         <v>0</v>
       </c>
       <c r="J282">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K282">
         <v>0</v>
@@ -15985,7 +15985,7 @@
         <v>0</v>
       </c>
       <c r="J283">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K283">
         <v>0</v>
@@ -16032,7 +16032,7 @@
         <v>0</v>
       </c>
       <c r="J284">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K284">
         <v>0</v>
@@ -16079,7 +16079,7 @@
         <v>0</v>
       </c>
       <c r="J285">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K285">
         <v>0</v>
@@ -16126,7 +16126,7 @@
         <v>0</v>
       </c>
       <c r="J286">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K286">
         <v>0</v>
@@ -16261,7 +16261,7 @@
         <v>0</v>
       </c>
       <c r="J289">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K289">
         <v>0</v>
@@ -16352,7 +16352,7 @@
         <v>0</v>
       </c>
       <c r="J291">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K291">
         <v>0</v>
@@ -16399,7 +16399,7 @@
         <v>0</v>
       </c>
       <c r="J292">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K292">
         <v>0</v>
@@ -16446,7 +16446,7 @@
         <v>0</v>
       </c>
       <c r="J293">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K293">
         <v>0</v>
@@ -16537,7 +16537,7 @@
         <v>0</v>
       </c>
       <c r="J295">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K295">
         <v>0</v>
@@ -16584,7 +16584,7 @@
         <v>0</v>
       </c>
       <c r="J296">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K296">
         <v>0</v>
@@ -16631,7 +16631,7 @@
         <v>0</v>
       </c>
       <c r="J297">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K297">
         <v>0</v>
@@ -16678,7 +16678,7 @@
         <v>0</v>
       </c>
       <c r="J298">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K298">
         <v>0</v>
@@ -16725,7 +16725,7 @@
         <v>0</v>
       </c>
       <c r="J299">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K299">
         <v>0</v>
@@ -16772,7 +16772,7 @@
         <v>0</v>
       </c>
       <c r="J300">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K300">
         <v>0</v>
@@ -16819,7 +16819,7 @@
         <v>0</v>
       </c>
       <c r="J301">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K301">
         <v>0</v>
@@ -16866,7 +16866,7 @@
         <v>0</v>
       </c>
       <c r="J302">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K302">
         <v>0</v>
@@ -16913,7 +16913,7 @@
         <v>0</v>
       </c>
       <c r="J303">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K303">
         <v>0</v>
@@ -16960,7 +16960,7 @@
         <v>0</v>
       </c>
       <c r="J304">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K304">
         <v>0</v>
@@ -17007,7 +17007,7 @@
         <v>0</v>
       </c>
       <c r="J305">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K305">
         <v>0</v>
@@ -17054,7 +17054,7 @@
         <v>0</v>
       </c>
       <c r="J306">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K306">
         <v>0</v>
@@ -17101,7 +17101,7 @@
         <v>0</v>
       </c>
       <c r="J307">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K307">
         <v>0</v>
@@ -17148,7 +17148,7 @@
         <v>0</v>
       </c>
       <c r="J308">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K308">
         <v>0</v>
@@ -17195,7 +17195,7 @@
         <v>0</v>
       </c>
       <c r="J309">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K309">
         <v>0</v>
@@ -17242,7 +17242,7 @@
         <v>0</v>
       </c>
       <c r="J310">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K310">
         <v>0</v>
@@ -17333,7 +17333,7 @@
         <v>0</v>
       </c>
       <c r="J312">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K312">
         <v>0</v>
@@ -17380,7 +17380,7 @@
         <v>0</v>
       </c>
       <c r="J313">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K313">
         <v>0</v>
@@ -17427,7 +17427,7 @@
         <v>0</v>
       </c>
       <c r="J314">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K314">
         <v>0</v>
@@ -17474,7 +17474,7 @@
         <v>0</v>
       </c>
       <c r="J315">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K315">
         <v>0</v>
@@ -17521,7 +17521,7 @@
         <v>0</v>
       </c>
       <c r="J316">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K316">
         <v>0</v>
@@ -17568,7 +17568,7 @@
         <v>0</v>
       </c>
       <c r="J317">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K317">
         <v>0</v>
@@ -17615,7 +17615,7 @@
         <v>0</v>
       </c>
       <c r="J318">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K318">
         <v>0</v>
@@ -17662,7 +17662,7 @@
         <v>0</v>
       </c>
       <c r="J319">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K319">
         <v>0</v>
@@ -17709,7 +17709,7 @@
         <v>0</v>
       </c>
       <c r="J320">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K320">
         <v>0</v>
@@ -17800,7 +17800,7 @@
         <v>0</v>
       </c>
       <c r="J322">
-        <v>1586659823.314746</v>
+        <v>1586660079.314404</v>
       </c>
       <c r="K322">
         <v>0</v>

</xml_diff>

<commit_message>
correct a viplevel bug
</commit_message>
<xml_diff>
--- a/CheckData.xlsx
+++ b/CheckData.xlsx
@@ -3039,7 +3039,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -3174,7 +3174,7 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -3221,7 +3221,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -3268,7 +3268,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -3359,7 +3359,7 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -3556,7 +3556,7 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -3653,7 +3653,7 @@
         <v>0</v>
       </c>
       <c r="J15">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K15">
         <v>0</v>
@@ -3750,7 +3750,7 @@
         <v>0</v>
       </c>
       <c r="J17">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K17">
         <v>0</v>
@@ -3797,7 +3797,7 @@
         <v>0</v>
       </c>
       <c r="J18">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K18">
         <v>0</v>
@@ -3844,7 +3844,7 @@
         <v>0</v>
       </c>
       <c r="J19">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K19">
         <v>0</v>
@@ -3985,7 +3985,7 @@
         <v>0</v>
       </c>
       <c r="J22">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K22">
         <v>0</v>
@@ -4164,7 +4164,7 @@
         <v>0</v>
       </c>
       <c r="J26">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K26">
         <v>0</v>
@@ -4211,7 +4211,7 @@
         <v>0</v>
       </c>
       <c r="J27">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K27">
         <v>0</v>
@@ -4302,7 +4302,7 @@
         <v>0</v>
       </c>
       <c r="J29">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K29">
         <v>0</v>
@@ -4349,7 +4349,7 @@
         <v>0</v>
       </c>
       <c r="J30">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K30">
         <v>0</v>
@@ -4396,7 +4396,7 @@
         <v>0</v>
       </c>
       <c r="J31">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K31">
         <v>0</v>
@@ -4493,7 +4493,7 @@
         <v>0</v>
       </c>
       <c r="J33">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K33">
         <v>0</v>
@@ -4590,7 +4590,7 @@
         <v>0</v>
       </c>
       <c r="J35">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K35">
         <v>0</v>
@@ -4637,7 +4637,7 @@
         <v>0</v>
       </c>
       <c r="J36">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K36">
         <v>0</v>
@@ -4684,7 +4684,7 @@
         <v>0</v>
       </c>
       <c r="J37">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K37">
         <v>0</v>
@@ -4731,7 +4731,7 @@
         <v>0</v>
       </c>
       <c r="J38">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K38">
         <v>0</v>
@@ -4787,10 +4787,10 @@
         <v>491</v>
       </c>
       <c r="M39">
-        <v>208.9050000000001</v>
+        <v>130.53</v>
       </c>
       <c r="N39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O39">
         <v>30</v>
@@ -4828,7 +4828,7 @@
         <v>0</v>
       </c>
       <c r="J40">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K40">
         <v>0</v>
@@ -4875,7 +4875,7 @@
         <v>0</v>
       </c>
       <c r="J41">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K41">
         <v>0</v>
@@ -4922,7 +4922,7 @@
         <v>0</v>
       </c>
       <c r="J42">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K42">
         <v>0</v>
@@ -5069,7 +5069,7 @@
         <v>0</v>
       </c>
       <c r="J45">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K45">
         <v>0</v>
@@ -5116,7 +5116,7 @@
         <v>0</v>
       </c>
       <c r="J46">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K46">
         <v>0</v>
@@ -5163,7 +5163,7 @@
         <v>0</v>
       </c>
       <c r="J47">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K47">
         <v>0</v>
@@ -5210,7 +5210,7 @@
         <v>0</v>
       </c>
       <c r="J48">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K48">
         <v>0</v>
@@ -5357,7 +5357,7 @@
         <v>0</v>
       </c>
       <c r="J51">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K51">
         <v>0</v>
@@ -5451,7 +5451,7 @@
         <v>0</v>
       </c>
       <c r="J53">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K53">
         <v>0</v>
@@ -5498,7 +5498,7 @@
         <v>0</v>
       </c>
       <c r="J54">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K54">
         <v>0</v>
@@ -5545,7 +5545,7 @@
         <v>0</v>
       </c>
       <c r="J55">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K55">
         <v>0</v>
@@ -5592,7 +5592,7 @@
         <v>0</v>
       </c>
       <c r="J56">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K56">
         <v>0</v>
@@ -5639,7 +5639,7 @@
         <v>0</v>
       </c>
       <c r="J57">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K57">
         <v>0</v>
@@ -5733,7 +5733,7 @@
         <v>0</v>
       </c>
       <c r="J59">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K59">
         <v>0</v>
@@ -5780,7 +5780,7 @@
         <v>0</v>
       </c>
       <c r="J60">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K60">
         <v>0</v>
@@ -5877,7 +5877,7 @@
         <v>0</v>
       </c>
       <c r="J62">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K62">
         <v>0</v>
@@ -5924,7 +5924,7 @@
         <v>0</v>
       </c>
       <c r="J63">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K63">
         <v>0</v>
@@ -6221,7 +6221,7 @@
         <v>0</v>
       </c>
       <c r="J69">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K69">
         <v>0</v>
@@ -6268,7 +6268,7 @@
         <v>0</v>
       </c>
       <c r="J70">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K70">
         <v>0</v>
@@ -6315,7 +6315,7 @@
         <v>0</v>
       </c>
       <c r="J71">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K71">
         <v>0</v>
@@ -6362,7 +6362,7 @@
         <v>0</v>
       </c>
       <c r="J72">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K72">
         <v>0</v>
@@ -6409,7 +6409,7 @@
         <v>0</v>
       </c>
       <c r="J73">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K73">
         <v>0</v>
@@ -6506,7 +6506,7 @@
         <v>0</v>
       </c>
       <c r="J75">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K75">
         <v>0</v>
@@ -6553,7 +6553,7 @@
         <v>0</v>
       </c>
       <c r="J76">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K76">
         <v>0</v>
@@ -6600,7 +6600,7 @@
         <v>0</v>
       </c>
       <c r="J77">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K77">
         <v>0</v>
@@ -6647,7 +6647,7 @@
         <v>0</v>
       </c>
       <c r="J78">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K78">
         <v>0</v>
@@ -6694,7 +6694,7 @@
         <v>0</v>
       </c>
       <c r="J79">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K79">
         <v>0</v>
@@ -6741,7 +6741,7 @@
         <v>0</v>
       </c>
       <c r="J80">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K80">
         <v>0</v>
@@ -6832,7 +6832,7 @@
         <v>0</v>
       </c>
       <c r="J82">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K82">
         <v>0</v>
@@ -7023,7 +7023,7 @@
         <v>0</v>
       </c>
       <c r="J86">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K86">
         <v>0</v>
@@ -7070,7 +7070,7 @@
         <v>0</v>
       </c>
       <c r="J87">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K87">
         <v>0</v>
@@ -7117,7 +7117,7 @@
         <v>0</v>
       </c>
       <c r="J88">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K88">
         <v>0</v>
@@ -7164,7 +7164,7 @@
         <v>0</v>
       </c>
       <c r="J89">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K89">
         <v>0</v>
@@ -7211,7 +7211,7 @@
         <v>0</v>
       </c>
       <c r="J90">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K90">
         <v>0</v>
@@ -7258,7 +7258,7 @@
         <v>0</v>
       </c>
       <c r="J91">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K91">
         <v>0</v>
@@ -7364,7 +7364,7 @@
         <v>545</v>
       </c>
       <c r="M93">
-        <v>360.6999999999999</v>
+        <v>372.7</v>
       </c>
       <c r="N93">
         <v>1</v>
@@ -7455,7 +7455,7 @@
         <v>0</v>
       </c>
       <c r="J95">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K95">
         <v>0</v>
@@ -7502,7 +7502,7 @@
         <v>0</v>
       </c>
       <c r="J96">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K96">
         <v>0</v>
@@ -7549,7 +7549,7 @@
         <v>0</v>
       </c>
       <c r="J97">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K97">
         <v>0</v>
@@ -7596,7 +7596,7 @@
         <v>0</v>
       </c>
       <c r="J98">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K98">
         <v>0</v>
@@ -7687,7 +7687,7 @@
         <v>0</v>
       </c>
       <c r="J100">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K100">
         <v>0</v>
@@ -7734,7 +7734,7 @@
         <v>0</v>
       </c>
       <c r="J101">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K101">
         <v>0</v>
@@ -7781,7 +7781,7 @@
         <v>0</v>
       </c>
       <c r="J102">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K102">
         <v>0</v>
@@ -7828,7 +7828,7 @@
         <v>0</v>
       </c>
       <c r="J103">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K103">
         <v>0</v>
@@ -7875,7 +7875,7 @@
         <v>0</v>
       </c>
       <c r="J104">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K104">
         <v>0</v>
@@ -7922,7 +7922,7 @@
         <v>0</v>
       </c>
       <c r="J105">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K105">
         <v>0</v>
@@ -7969,7 +7969,7 @@
         <v>0</v>
       </c>
       <c r="J106">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K106">
         <v>0</v>
@@ -8060,7 +8060,7 @@
         <v>0</v>
       </c>
       <c r="J108">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K108">
         <v>0</v>
@@ -8107,7 +8107,7 @@
         <v>0</v>
       </c>
       <c r="J109">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K109">
         <v>0</v>
@@ -8154,7 +8154,7 @@
         <v>0</v>
       </c>
       <c r="J110">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K110">
         <v>0</v>
@@ -8201,7 +8201,7 @@
         <v>0</v>
       </c>
       <c r="J111">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K111">
         <v>0</v>
@@ -8248,7 +8248,7 @@
         <v>0</v>
       </c>
       <c r="J112">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K112">
         <v>0</v>
@@ -8295,7 +8295,7 @@
         <v>0</v>
       </c>
       <c r="J113">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K113">
         <v>0</v>
@@ -8430,7 +8430,7 @@
         <v>0</v>
       </c>
       <c r="J116">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K116">
         <v>0</v>
@@ -8477,7 +8477,7 @@
         <v>0</v>
       </c>
       <c r="J117">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K117">
         <v>0</v>
@@ -8712,7 +8712,7 @@
         <v>0</v>
       </c>
       <c r="J122">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K122">
         <v>0</v>
@@ -8809,7 +8809,7 @@
         <v>0</v>
       </c>
       <c r="J124">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K124">
         <v>0</v>
@@ -8856,7 +8856,7 @@
         <v>0</v>
       </c>
       <c r="J125">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K125">
         <v>0</v>
@@ -8903,7 +8903,7 @@
         <v>0</v>
       </c>
       <c r="J126">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K126">
         <v>0</v>
@@ -8950,7 +8950,7 @@
         <v>0</v>
       </c>
       <c r="J127">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K127">
         <v>0</v>
@@ -8997,7 +8997,7 @@
         <v>0</v>
       </c>
       <c r="J128">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K128">
         <v>0</v>
@@ -9044,7 +9044,7 @@
         <v>0</v>
       </c>
       <c r="J129">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K129">
         <v>0</v>
@@ -9091,7 +9091,7 @@
         <v>0</v>
       </c>
       <c r="J130">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K130">
         <v>0</v>
@@ -9138,7 +9138,7 @@
         <v>0</v>
       </c>
       <c r="J131">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K131">
         <v>0</v>
@@ -9185,7 +9185,7 @@
         <v>0</v>
       </c>
       <c r="J132">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K132">
         <v>0</v>
@@ -9382,7 +9382,7 @@
         <v>0</v>
       </c>
       <c r="J136">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K136">
         <v>0</v>
@@ -9429,7 +9429,7 @@
         <v>0</v>
       </c>
       <c r="J137">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K137">
         <v>0</v>
@@ -9476,7 +9476,7 @@
         <v>0</v>
       </c>
       <c r="J138">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K138">
         <v>0</v>
@@ -9523,7 +9523,7 @@
         <v>0</v>
       </c>
       <c r="J139">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K139">
         <v>0</v>
@@ -9570,7 +9570,7 @@
         <v>0</v>
       </c>
       <c r="J140">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K140">
         <v>0</v>
@@ -9617,7 +9617,7 @@
         <v>0</v>
       </c>
       <c r="J141">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K141">
         <v>0</v>
@@ -9664,7 +9664,7 @@
         <v>0</v>
       </c>
       <c r="J142">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K142">
         <v>0</v>
@@ -9711,7 +9711,7 @@
         <v>0</v>
       </c>
       <c r="J143">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K143">
         <v>0</v>
@@ -9758,7 +9758,7 @@
         <v>0</v>
       </c>
       <c r="J144">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K144">
         <v>0</v>
@@ -9805,7 +9805,7 @@
         <v>0</v>
       </c>
       <c r="J145">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K145">
         <v>0</v>
@@ -9902,16 +9902,16 @@
         <v>0</v>
       </c>
       <c r="J147">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K147">
         <v>0</v>
       </c>
       <c r="M147">
-        <v>78.70000000000003</v>
+        <v>0</v>
       </c>
       <c r="N147">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O147">
         <v>0</v>
@@ -10043,7 +10043,7 @@
         <v>0</v>
       </c>
       <c r="J150">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K150">
         <v>0</v>
@@ -10090,7 +10090,7 @@
         <v>0</v>
       </c>
       <c r="J151">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K151">
         <v>0</v>
@@ -10137,7 +10137,7 @@
         <v>0</v>
       </c>
       <c r="J152">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K152">
         <v>0</v>
@@ -10184,7 +10184,7 @@
         <v>0</v>
       </c>
       <c r="J153">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K153">
         <v>0</v>
@@ -10275,7 +10275,7 @@
         <v>0</v>
       </c>
       <c r="J155">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K155">
         <v>0</v>
@@ -10322,7 +10322,7 @@
         <v>0</v>
       </c>
       <c r="J156">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K156">
         <v>0</v>
@@ -10369,7 +10369,7 @@
         <v>0</v>
       </c>
       <c r="J157">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K157">
         <v>0</v>
@@ -10416,7 +10416,7 @@
         <v>0</v>
       </c>
       <c r="J158">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K158">
         <v>0</v>
@@ -10463,7 +10463,7 @@
         <v>0</v>
       </c>
       <c r="J159">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K159">
         <v>0</v>
@@ -10510,7 +10510,7 @@
         <v>0</v>
       </c>
       <c r="J160">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K160">
         <v>0</v>
@@ -10557,7 +10557,7 @@
         <v>0</v>
       </c>
       <c r="J161">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K161">
         <v>0</v>
@@ -10604,7 +10604,7 @@
         <v>0</v>
       </c>
       <c r="J162">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K162">
         <v>0</v>
@@ -10751,7 +10751,7 @@
         <v>0</v>
       </c>
       <c r="J165">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K165">
         <v>0</v>
@@ -10798,7 +10798,7 @@
         <v>0</v>
       </c>
       <c r="J166">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K166">
         <v>0</v>
@@ -10845,7 +10845,7 @@
         <v>0</v>
       </c>
       <c r="J167">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K167">
         <v>0</v>
@@ -10936,7 +10936,7 @@
         <v>0</v>
       </c>
       <c r="J169">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K169">
         <v>0</v>
@@ -10983,7 +10983,7 @@
         <v>0</v>
       </c>
       <c r="J170">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K170">
         <v>0</v>
@@ -11030,7 +11030,7 @@
         <v>0</v>
       </c>
       <c r="J171">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K171">
         <v>0</v>
@@ -11077,7 +11077,7 @@
         <v>0</v>
       </c>
       <c r="J172">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K172">
         <v>0</v>
@@ -11124,7 +11124,7 @@
         <v>0</v>
       </c>
       <c r="J173">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K173">
         <v>0</v>
@@ -11171,7 +11171,7 @@
         <v>0</v>
       </c>
       <c r="J174">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K174">
         <v>0</v>
@@ -11268,7 +11268,7 @@
         <v>0</v>
       </c>
       <c r="J176">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K176">
         <v>0</v>
@@ -11315,7 +11315,7 @@
         <v>0</v>
       </c>
       <c r="J177">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K177">
         <v>0</v>
@@ -11362,7 +11362,7 @@
         <v>0</v>
       </c>
       <c r="J178">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K178">
         <v>0</v>
@@ -11509,7 +11509,7 @@
         <v>0</v>
       </c>
       <c r="J181">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K181">
         <v>0</v>
@@ -11650,7 +11650,7 @@
         <v>0</v>
       </c>
       <c r="J184">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K184">
         <v>0</v>
@@ -11747,7 +11747,7 @@
         <v>0</v>
       </c>
       <c r="J186">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K186">
         <v>0</v>
@@ -11888,7 +11888,7 @@
         <v>0</v>
       </c>
       <c r="J189">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K189">
         <v>0</v>
@@ -11935,7 +11935,7 @@
         <v>0</v>
       </c>
       <c r="J190">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K190">
         <v>0</v>
@@ -11982,7 +11982,7 @@
         <v>0</v>
       </c>
       <c r="J191">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K191">
         <v>0</v>
@@ -12029,7 +12029,7 @@
         <v>0</v>
       </c>
       <c r="J192">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K192">
         <v>0</v>
@@ -12126,7 +12126,7 @@
         <v>0</v>
       </c>
       <c r="J194">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K194">
         <v>0</v>
@@ -12173,7 +12173,7 @@
         <v>0</v>
       </c>
       <c r="J195">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K195">
         <v>0</v>
@@ -12264,7 +12264,7 @@
         <v>0</v>
       </c>
       <c r="J197">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K197">
         <v>0</v>
@@ -12311,7 +12311,7 @@
         <v>0</v>
       </c>
       <c r="J198">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K198">
         <v>0</v>
@@ -12358,7 +12358,7 @@
         <v>0</v>
       </c>
       <c r="J199">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K199">
         <v>0</v>
@@ -12405,7 +12405,7 @@
         <v>0</v>
       </c>
       <c r="J200">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K200">
         <v>0</v>
@@ -12452,7 +12452,7 @@
         <v>0</v>
       </c>
       <c r="J201">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K201">
         <v>0</v>
@@ -12499,7 +12499,7 @@
         <v>0</v>
       </c>
       <c r="J202">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K202">
         <v>0</v>
@@ -12546,7 +12546,7 @@
         <v>0</v>
       </c>
       <c r="J203">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K203">
         <v>0</v>
@@ -12637,7 +12637,7 @@
         <v>0</v>
       </c>
       <c r="J205">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K205">
         <v>0</v>
@@ -12734,7 +12734,7 @@
         <v>0</v>
       </c>
       <c r="J207">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K207">
         <v>0</v>
@@ -12825,7 +12825,7 @@
         <v>0</v>
       </c>
       <c r="J209">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K209">
         <v>0</v>
@@ -12922,7 +12922,7 @@
         <v>0</v>
       </c>
       <c r="J211">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K211">
         <v>0</v>
@@ -12969,7 +12969,7 @@
         <v>0</v>
       </c>
       <c r="J212">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K212">
         <v>0</v>
@@ -13016,7 +13016,7 @@
         <v>0</v>
       </c>
       <c r="J213">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K213">
         <v>0</v>
@@ -13063,7 +13063,7 @@
         <v>0</v>
       </c>
       <c r="J214">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K214">
         <v>0</v>
@@ -13110,7 +13110,7 @@
         <v>0</v>
       </c>
       <c r="J215">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K215">
         <v>0</v>
@@ -13157,7 +13157,7 @@
         <v>0</v>
       </c>
       <c r="J216">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K216">
         <v>0</v>
@@ -13204,7 +13204,7 @@
         <v>0</v>
       </c>
       <c r="J217">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K217">
         <v>0</v>
@@ -13251,7 +13251,7 @@
         <v>0</v>
       </c>
       <c r="J218">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K218">
         <v>0</v>
@@ -13298,7 +13298,7 @@
         <v>0</v>
       </c>
       <c r="J219">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K219">
         <v>0</v>
@@ -13395,7 +13395,7 @@
         <v>0</v>
       </c>
       <c r="J221">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K221">
         <v>0</v>
@@ -13442,7 +13442,7 @@
         <v>0</v>
       </c>
       <c r="J222">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K222">
         <v>0</v>
@@ -13489,7 +13489,7 @@
         <v>0</v>
       </c>
       <c r="J223">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K223">
         <v>0</v>
@@ -13545,10 +13545,10 @@
         <v>676</v>
       </c>
       <c r="M224">
-        <v>175.6000000000001</v>
+        <v>90</v>
       </c>
       <c r="N224">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O224">
         <v>30</v>
@@ -13680,7 +13680,7 @@
         <v>0</v>
       </c>
       <c r="J227">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K227">
         <v>0</v>
@@ -13736,7 +13736,7 @@
         <v>680</v>
       </c>
       <c r="M228">
-        <v>181.2</v>
+        <v>193.2795</v>
       </c>
       <c r="N228">
         <v>1</v>
@@ -13777,7 +13777,7 @@
         <v>0</v>
       </c>
       <c r="J229">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K229">
         <v>0</v>
@@ -13918,7 +13918,7 @@
         <v>0</v>
       </c>
       <c r="J232">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K232">
         <v>0</v>
@@ -13965,7 +13965,7 @@
         <v>0</v>
       </c>
       <c r="J233">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K233">
         <v>0</v>
@@ -14012,7 +14012,7 @@
         <v>0</v>
       </c>
       <c r="J234">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K234">
         <v>0</v>
@@ -14059,7 +14059,7 @@
         <v>0</v>
       </c>
       <c r="J235">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K235">
         <v>0</v>
@@ -14156,7 +14156,7 @@
         <v>0</v>
       </c>
       <c r="J237">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K237">
         <v>0</v>
@@ -14203,7 +14203,7 @@
         <v>0</v>
       </c>
       <c r="J238">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K238">
         <v>0</v>
@@ -14250,7 +14250,7 @@
         <v>0</v>
       </c>
       <c r="J239">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K239">
         <v>0</v>
@@ -14297,7 +14297,7 @@
         <v>0</v>
       </c>
       <c r="J240">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K240">
         <v>0</v>
@@ -14344,7 +14344,7 @@
         <v>0</v>
       </c>
       <c r="J241">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K241">
         <v>0</v>
@@ -14391,7 +14391,7 @@
         <v>0</v>
       </c>
       <c r="J242">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K242">
         <v>0</v>
@@ -14482,7 +14482,7 @@
         <v>0</v>
       </c>
       <c r="J244">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K244">
         <v>0</v>
@@ -14529,7 +14529,7 @@
         <v>0</v>
       </c>
       <c r="J245">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K245">
         <v>0</v>
@@ -14576,7 +14576,7 @@
         <v>0</v>
       </c>
       <c r="J246">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K246">
         <v>0</v>
@@ -14623,7 +14623,7 @@
         <v>0</v>
       </c>
       <c r="J247">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K247">
         <v>0</v>
@@ -14670,7 +14670,7 @@
         <v>0</v>
       </c>
       <c r="J248">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K248">
         <v>0</v>
@@ -14767,7 +14767,7 @@
         <v>0</v>
       </c>
       <c r="J250">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K250">
         <v>0</v>
@@ -14814,7 +14814,7 @@
         <v>0</v>
       </c>
       <c r="J251">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K251">
         <v>0</v>
@@ -14861,7 +14861,7 @@
         <v>0</v>
       </c>
       <c r="J252">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K252">
         <v>0</v>
@@ -14908,7 +14908,7 @@
         <v>0</v>
       </c>
       <c r="J253">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K253">
         <v>0</v>
@@ -14999,7 +14999,7 @@
         <v>0</v>
       </c>
       <c r="J255">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K255">
         <v>0</v>
@@ -15046,7 +15046,7 @@
         <v>0</v>
       </c>
       <c r="J256">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K256">
         <v>0</v>
@@ -15093,7 +15093,7 @@
         <v>0</v>
       </c>
       <c r="J257">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K257">
         <v>0</v>
@@ -15284,7 +15284,7 @@
         <v>0</v>
       </c>
       <c r="J261">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K261">
         <v>0</v>
@@ -15331,7 +15331,7 @@
         <v>0</v>
       </c>
       <c r="J262">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K262">
         <v>0</v>
@@ -15378,7 +15378,7 @@
         <v>0</v>
       </c>
       <c r="J263">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K263">
         <v>0</v>
@@ -15469,7 +15469,7 @@
         <v>0</v>
       </c>
       <c r="J265">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K265">
         <v>0</v>
@@ -15716,7 +15716,7 @@
         <v>0</v>
       </c>
       <c r="J270">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K270">
         <v>0</v>
@@ -15763,7 +15763,7 @@
         <v>0</v>
       </c>
       <c r="J271">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K271">
         <v>0</v>
@@ -15810,7 +15810,7 @@
         <v>0</v>
       </c>
       <c r="J272">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K272">
         <v>0</v>
@@ -15857,7 +15857,7 @@
         <v>0</v>
       </c>
       <c r="J273">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K273">
         <v>0</v>
@@ -15904,7 +15904,7 @@
         <v>0</v>
       </c>
       <c r="J274">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K274">
         <v>0</v>
@@ -15951,7 +15951,7 @@
         <v>0</v>
       </c>
       <c r="J275">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K275">
         <v>0</v>
@@ -16042,7 +16042,7 @@
         <v>0</v>
       </c>
       <c r="J277">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K277">
         <v>0</v>
@@ -16139,7 +16139,7 @@
         <v>0</v>
       </c>
       <c r="J279">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K279">
         <v>0</v>
@@ -16186,7 +16186,7 @@
         <v>0</v>
       </c>
       <c r="J280">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K280">
         <v>0</v>
@@ -16283,7 +16283,7 @@
         <v>0</v>
       </c>
       <c r="J282">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K282">
         <v>0</v>
@@ -16380,7 +16380,7 @@
         <v>0</v>
       </c>
       <c r="J284">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K284">
         <v>0</v>
@@ -16477,7 +16477,7 @@
         <v>0</v>
       </c>
       <c r="J286">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K286">
         <v>0</v>
@@ -16574,7 +16574,7 @@
         <v>0</v>
       </c>
       <c r="J288">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K288">
         <v>0</v>
@@ -16621,7 +16621,7 @@
         <v>0</v>
       </c>
       <c r="J289">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K289">
         <v>0</v>
@@ -16668,7 +16668,7 @@
         <v>0</v>
       </c>
       <c r="J290">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K290">
         <v>0</v>
@@ -16715,7 +16715,7 @@
         <v>0</v>
       </c>
       <c r="J291">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K291">
         <v>0</v>
@@ -16762,7 +16762,7 @@
         <v>0</v>
       </c>
       <c r="J292">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K292">
         <v>0</v>
@@ -16859,7 +16859,7 @@
         <v>0</v>
       </c>
       <c r="J294">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K294">
         <v>0</v>
@@ -16956,7 +16956,7 @@
         <v>0</v>
       </c>
       <c r="J296">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K296">
         <v>0</v>
@@ -17053,7 +17053,7 @@
         <v>0</v>
       </c>
       <c r="J298">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K298">
         <v>0</v>
@@ -17100,7 +17100,7 @@
         <v>0</v>
       </c>
       <c r="J299">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K299">
         <v>0</v>
@@ -17147,7 +17147,7 @@
         <v>0</v>
       </c>
       <c r="J300">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K300">
         <v>0</v>
@@ -17294,7 +17294,7 @@
         <v>0</v>
       </c>
       <c r="J303">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K303">
         <v>0</v>
@@ -17341,7 +17341,7 @@
         <v>0</v>
       </c>
       <c r="J304">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K304">
         <v>0</v>
@@ -17388,7 +17388,7 @@
         <v>0</v>
       </c>
       <c r="J305">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K305">
         <v>0</v>
@@ -17435,7 +17435,7 @@
         <v>0</v>
       </c>
       <c r="J306">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K306">
         <v>0</v>
@@ -17526,7 +17526,7 @@
         <v>0</v>
       </c>
       <c r="J308">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K308">
         <v>0</v>
@@ -17623,7 +17623,7 @@
         <v>0</v>
       </c>
       <c r="J310">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K310">
         <v>0</v>
@@ -17670,7 +17670,7 @@
         <v>0</v>
       </c>
       <c r="J311">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K311">
         <v>0</v>
@@ -17717,7 +17717,7 @@
         <v>0</v>
       </c>
       <c r="J312">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K312">
         <v>0</v>
@@ -17955,7 +17955,7 @@
         <v>0</v>
       </c>
       <c r="J317">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K317">
         <v>0</v>
@@ -18052,7 +18052,7 @@
         <v>0</v>
       </c>
       <c r="J319">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K319">
         <v>0</v>
@@ -18149,7 +18149,7 @@
         <v>0</v>
       </c>
       <c r="J321">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K321">
         <v>0</v>
@@ -18196,7 +18196,7 @@
         <v>0</v>
       </c>
       <c r="J322">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K322">
         <v>0</v>
@@ -18287,7 +18287,7 @@
         <v>0</v>
       </c>
       <c r="J324">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K324">
         <v>0</v>
@@ -18334,7 +18334,7 @@
         <v>0</v>
       </c>
       <c r="J325">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K325">
         <v>0</v>
@@ -18381,7 +18381,7 @@
         <v>0</v>
       </c>
       <c r="J326">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K326">
         <v>0</v>
@@ -18472,7 +18472,7 @@
         <v>0</v>
       </c>
       <c r="J328">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K328">
         <v>0</v>
@@ -18519,7 +18519,7 @@
         <v>0</v>
       </c>
       <c r="J329">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K329">
         <v>0</v>
@@ -18566,7 +18566,7 @@
         <v>0</v>
       </c>
       <c r="J330">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K330">
         <v>0</v>
@@ -18707,7 +18707,7 @@
         <v>0</v>
       </c>
       <c r="J333">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K333">
         <v>0</v>
@@ -18804,7 +18804,7 @@
         <v>0</v>
       </c>
       <c r="J335">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K335">
         <v>0</v>
@@ -18951,7 +18951,7 @@
         <v>0</v>
       </c>
       <c r="J338">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K338">
         <v>0</v>
@@ -19048,7 +19048,7 @@
         <v>0</v>
       </c>
       <c r="J340">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K340">
         <v>0</v>
@@ -19095,7 +19095,7 @@
         <v>0</v>
       </c>
       <c r="J341">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K341">
         <v>0</v>
@@ -19142,7 +19142,7 @@
         <v>0</v>
       </c>
       <c r="J342">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K342">
         <v>0</v>
@@ -19189,7 +19189,7 @@
         <v>0</v>
       </c>
       <c r="J343">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K343">
         <v>0</v>
@@ -19236,7 +19236,7 @@
         <v>0</v>
       </c>
       <c r="J344">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K344">
         <v>0</v>
@@ -19483,7 +19483,7 @@
         <v>0</v>
       </c>
       <c r="J349">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K349">
         <v>0</v>
@@ -19530,7 +19530,7 @@
         <v>0</v>
       </c>
       <c r="J350">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K350">
         <v>0</v>
@@ -19577,7 +19577,7 @@
         <v>0</v>
       </c>
       <c r="J351">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K351">
         <v>0</v>
@@ -19674,7 +19674,7 @@
         <v>0</v>
       </c>
       <c r="J353">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K353">
         <v>0</v>
@@ -19915,7 +19915,7 @@
         <v>0</v>
       </c>
       <c r="J358">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K358">
         <v>0</v>
@@ -19962,7 +19962,7 @@
         <v>0</v>
       </c>
       <c r="J359">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K359">
         <v>0</v>
@@ -20009,7 +20009,7 @@
         <v>0</v>
       </c>
       <c r="J360">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K360">
         <v>0</v>
@@ -20056,7 +20056,7 @@
         <v>0</v>
       </c>
       <c r="J361">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K361">
         <v>0</v>
@@ -20153,7 +20153,7 @@
         <v>0</v>
       </c>
       <c r="J363">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K363">
         <v>0</v>
@@ -20200,7 +20200,7 @@
         <v>0</v>
       </c>
       <c r="J364">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K364">
         <v>0</v>
@@ -20247,7 +20247,7 @@
         <v>0</v>
       </c>
       <c r="J365">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K365">
         <v>0</v>
@@ -20438,7 +20438,7 @@
         <v>0</v>
       </c>
       <c r="J369">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K369">
         <v>0</v>
@@ -20485,7 +20485,7 @@
         <v>0</v>
       </c>
       <c r="J370">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K370">
         <v>0</v>
@@ -20582,7 +20582,7 @@
         <v>0</v>
       </c>
       <c r="J372">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K372">
         <v>0</v>
@@ -20629,7 +20629,7 @@
         <v>0</v>
       </c>
       <c r="J373">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K373">
         <v>0</v>
@@ -20676,7 +20676,7 @@
         <v>0</v>
       </c>
       <c r="J374">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K374">
         <v>0</v>
@@ -20723,7 +20723,7 @@
         <v>0</v>
       </c>
       <c r="J375">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K375">
         <v>0</v>
@@ -20770,7 +20770,7 @@
         <v>0</v>
       </c>
       <c r="J376">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K376">
         <v>0</v>
@@ -20817,7 +20817,7 @@
         <v>0</v>
       </c>
       <c r="J377">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K377">
         <v>0</v>
@@ -20964,7 +20964,7 @@
         <v>0</v>
       </c>
       <c r="J380">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K380">
         <v>0</v>
@@ -21111,7 +21111,7 @@
         <v>0</v>
       </c>
       <c r="J383">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K383">
         <v>0</v>
@@ -21158,7 +21158,7 @@
         <v>0</v>
       </c>
       <c r="J384">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K384">
         <v>0</v>
@@ -21205,7 +21205,7 @@
         <v>0</v>
       </c>
       <c r="J385">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K385">
         <v>0</v>
@@ -21252,7 +21252,7 @@
         <v>0</v>
       </c>
       <c r="J386">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K386">
         <v>0</v>
@@ -21299,7 +21299,7 @@
         <v>0</v>
       </c>
       <c r="J387">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K387">
         <v>0</v>
@@ -21346,7 +21346,7 @@
         <v>0</v>
       </c>
       <c r="J388">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K388">
         <v>0</v>
@@ -21393,7 +21393,7 @@
         <v>0</v>
       </c>
       <c r="J389">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K389">
         <v>0</v>
@@ -21540,7 +21540,7 @@
         <v>0</v>
       </c>
       <c r="J392">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K392">
         <v>0</v>
@@ -21587,7 +21587,7 @@
         <v>0</v>
       </c>
       <c r="J393">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K393">
         <v>0</v>
@@ -21678,7 +21678,7 @@
         <v>0</v>
       </c>
       <c r="J395">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K395">
         <v>0</v>
@@ -21725,7 +21725,7 @@
         <v>0</v>
       </c>
       <c r="J396">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K396">
         <v>0</v>
@@ -21772,7 +21772,7 @@
         <v>0</v>
       </c>
       <c r="J397">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K397">
         <v>0</v>
@@ -21869,7 +21869,7 @@
         <v>0</v>
       </c>
       <c r="J399">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K399">
         <v>0</v>
@@ -21916,7 +21916,7 @@
         <v>0</v>
       </c>
       <c r="J400">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K400">
         <v>0</v>
@@ -21963,7 +21963,7 @@
         <v>0</v>
       </c>
       <c r="J401">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K401">
         <v>0</v>
@@ -22060,7 +22060,7 @@
         <v>0</v>
       </c>
       <c r="J403">
-        <v>1586862571.589257</v>
+        <v>1586918607.814806</v>
       </c>
       <c r="K403">
         <v>0</v>

</xml_diff>

<commit_message>
design js check version
</commit_message>
<xml_diff>
--- a/CheckData.xlsx
+++ b/CheckData.xlsx
@@ -3039,7 +3039,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -3174,7 +3174,7 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -3221,7 +3221,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -3268,7 +3268,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -3359,7 +3359,7 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -3556,7 +3556,7 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -3653,7 +3653,7 @@
         <v>0</v>
       </c>
       <c r="J15">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K15">
         <v>0</v>
@@ -3750,7 +3750,7 @@
         <v>0</v>
       </c>
       <c r="J17">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K17">
         <v>0</v>
@@ -3797,7 +3797,7 @@
         <v>0</v>
       </c>
       <c r="J18">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K18">
         <v>0</v>
@@ -3844,7 +3844,7 @@
         <v>0</v>
       </c>
       <c r="J19">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K19">
         <v>0</v>
@@ -3985,7 +3985,7 @@
         <v>0</v>
       </c>
       <c r="J22">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K22">
         <v>0</v>
@@ -4164,7 +4164,7 @@
         <v>0</v>
       </c>
       <c r="J26">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K26">
         <v>0</v>
@@ -4211,7 +4211,7 @@
         <v>0</v>
       </c>
       <c r="J27">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K27">
         <v>0</v>
@@ -4302,7 +4302,7 @@
         <v>0</v>
       </c>
       <c r="J29">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K29">
         <v>0</v>
@@ -4349,7 +4349,7 @@
         <v>0</v>
       </c>
       <c r="J30">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K30">
         <v>0</v>
@@ -4396,7 +4396,7 @@
         <v>0</v>
       </c>
       <c r="J31">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K31">
         <v>0</v>
@@ -4493,7 +4493,7 @@
         <v>0</v>
       </c>
       <c r="J33">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K33">
         <v>0</v>
@@ -4590,7 +4590,7 @@
         <v>0</v>
       </c>
       <c r="J35">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K35">
         <v>0</v>
@@ -4637,7 +4637,7 @@
         <v>0</v>
       </c>
       <c r="J36">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K36">
         <v>0</v>
@@ -4684,7 +4684,7 @@
         <v>0</v>
       </c>
       <c r="J37">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K37">
         <v>0</v>
@@ -4731,7 +4731,7 @@
         <v>0</v>
       </c>
       <c r="J38">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K38">
         <v>0</v>
@@ -4828,7 +4828,7 @@
         <v>0</v>
       </c>
       <c r="J40">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K40">
         <v>0</v>
@@ -4875,7 +4875,7 @@
         <v>0</v>
       </c>
       <c r="J41">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K41">
         <v>0</v>
@@ -4922,7 +4922,7 @@
         <v>0</v>
       </c>
       <c r="J42">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K42">
         <v>0</v>
@@ -5069,7 +5069,7 @@
         <v>0</v>
       </c>
       <c r="J45">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K45">
         <v>0</v>
@@ -5116,7 +5116,7 @@
         <v>0</v>
       </c>
       <c r="J46">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K46">
         <v>0</v>
@@ -5163,7 +5163,7 @@
         <v>0</v>
       </c>
       <c r="J47">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K47">
         <v>0</v>
@@ -5210,7 +5210,7 @@
         <v>0</v>
       </c>
       <c r="J48">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K48">
         <v>0</v>
@@ -5357,7 +5357,7 @@
         <v>0</v>
       </c>
       <c r="J51">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K51">
         <v>0</v>
@@ -5451,7 +5451,7 @@
         <v>0</v>
       </c>
       <c r="J53">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K53">
         <v>0</v>
@@ -5498,7 +5498,7 @@
         <v>0</v>
       </c>
       <c r="J54">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K54">
         <v>0</v>
@@ -5545,7 +5545,7 @@
         <v>0</v>
       </c>
       <c r="J55">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K55">
         <v>0</v>
@@ -5592,7 +5592,7 @@
         <v>0</v>
       </c>
       <c r="J56">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K56">
         <v>0</v>
@@ -5639,7 +5639,7 @@
         <v>0</v>
       </c>
       <c r="J57">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K57">
         <v>0</v>
@@ -5733,7 +5733,7 @@
         <v>0</v>
       </c>
       <c r="J59">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K59">
         <v>0</v>
@@ -5780,7 +5780,7 @@
         <v>0</v>
       </c>
       <c r="J60">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K60">
         <v>0</v>
@@ -5877,7 +5877,7 @@
         <v>0</v>
       </c>
       <c r="J62">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K62">
         <v>0</v>
@@ -5924,7 +5924,7 @@
         <v>0</v>
       </c>
       <c r="J63">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K63">
         <v>0</v>
@@ -6221,7 +6221,7 @@
         <v>0</v>
       </c>
       <c r="J69">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K69">
         <v>0</v>
@@ -6268,7 +6268,7 @@
         <v>0</v>
       </c>
       <c r="J70">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K70">
         <v>0</v>
@@ -6315,7 +6315,7 @@
         <v>0</v>
       </c>
       <c r="J71">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K71">
         <v>0</v>
@@ -6362,7 +6362,7 @@
         <v>0</v>
       </c>
       <c r="J72">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K72">
         <v>0</v>
@@ -6409,7 +6409,7 @@
         <v>0</v>
       </c>
       <c r="J73">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K73">
         <v>0</v>
@@ -6506,7 +6506,7 @@
         <v>0</v>
       </c>
       <c r="J75">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K75">
         <v>0</v>
@@ -6553,7 +6553,7 @@
         <v>0</v>
       </c>
       <c r="J76">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K76">
         <v>0</v>
@@ -6600,7 +6600,7 @@
         <v>0</v>
       </c>
       <c r="J77">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K77">
         <v>0</v>
@@ -6647,7 +6647,7 @@
         <v>0</v>
       </c>
       <c r="J78">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K78">
         <v>0</v>
@@ -6694,7 +6694,7 @@
         <v>0</v>
       </c>
       <c r="J79">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K79">
         <v>0</v>
@@ -6741,7 +6741,7 @@
         <v>0</v>
       </c>
       <c r="J80">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K80">
         <v>0</v>
@@ -6832,7 +6832,7 @@
         <v>0</v>
       </c>
       <c r="J82">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K82">
         <v>0</v>
@@ -7023,7 +7023,7 @@
         <v>0</v>
       </c>
       <c r="J86">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K86">
         <v>0</v>
@@ -7070,7 +7070,7 @@
         <v>0</v>
       </c>
       <c r="J87">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K87">
         <v>0</v>
@@ -7117,7 +7117,7 @@
         <v>0</v>
       </c>
       <c r="J88">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K88">
         <v>0</v>
@@ -7164,7 +7164,7 @@
         <v>0</v>
       </c>
       <c r="J89">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K89">
         <v>0</v>
@@ -7211,7 +7211,7 @@
         <v>0</v>
       </c>
       <c r="J90">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K90">
         <v>0</v>
@@ -7258,7 +7258,7 @@
         <v>0</v>
       </c>
       <c r="J91">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K91">
         <v>0</v>
@@ -7455,7 +7455,7 @@
         <v>0</v>
       </c>
       <c r="J95">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K95">
         <v>0</v>
@@ -7502,7 +7502,7 @@
         <v>0</v>
       </c>
       <c r="J96">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K96">
         <v>0</v>
@@ -7549,7 +7549,7 @@
         <v>0</v>
       </c>
       <c r="J97">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K97">
         <v>0</v>
@@ -7596,7 +7596,7 @@
         <v>0</v>
       </c>
       <c r="J98">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K98">
         <v>0</v>
@@ -7687,7 +7687,7 @@
         <v>0</v>
       </c>
       <c r="J100">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K100">
         <v>0</v>
@@ -7734,7 +7734,7 @@
         <v>0</v>
       </c>
       <c r="J101">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K101">
         <v>0</v>
@@ -7781,7 +7781,7 @@
         <v>0</v>
       </c>
       <c r="J102">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K102">
         <v>0</v>
@@ -7828,7 +7828,7 @@
         <v>0</v>
       </c>
       <c r="J103">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K103">
         <v>0</v>
@@ -7875,7 +7875,7 @@
         <v>0</v>
       </c>
       <c r="J104">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K104">
         <v>0</v>
@@ -7922,7 +7922,7 @@
         <v>0</v>
       </c>
       <c r="J105">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K105">
         <v>0</v>
@@ -7969,7 +7969,7 @@
         <v>0</v>
       </c>
       <c r="J106">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K106">
         <v>0</v>
@@ -8060,7 +8060,7 @@
         <v>0</v>
       </c>
       <c r="J108">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K108">
         <v>0</v>
@@ -8107,7 +8107,7 @@
         <v>0</v>
       </c>
       <c r="J109">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K109">
         <v>0</v>
@@ -8154,7 +8154,7 @@
         <v>0</v>
       </c>
       <c r="J110">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K110">
         <v>0</v>
@@ -8201,7 +8201,7 @@
         <v>0</v>
       </c>
       <c r="J111">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K111">
         <v>0</v>
@@ -8248,7 +8248,7 @@
         <v>0</v>
       </c>
       <c r="J112">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K112">
         <v>0</v>
@@ -8295,7 +8295,7 @@
         <v>0</v>
       </c>
       <c r="J113">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K113">
         <v>0</v>
@@ -8430,7 +8430,7 @@
         <v>0</v>
       </c>
       <c r="J116">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K116">
         <v>0</v>
@@ -8477,7 +8477,7 @@
         <v>0</v>
       </c>
       <c r="J117">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K117">
         <v>0</v>
@@ -8712,7 +8712,7 @@
         <v>0</v>
       </c>
       <c r="J122">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K122">
         <v>0</v>
@@ -8809,7 +8809,7 @@
         <v>0</v>
       </c>
       <c r="J124">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K124">
         <v>0</v>
@@ -8856,7 +8856,7 @@
         <v>0</v>
       </c>
       <c r="J125">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K125">
         <v>0</v>
@@ -8903,7 +8903,7 @@
         <v>0</v>
       </c>
       <c r="J126">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K126">
         <v>0</v>
@@ -8950,7 +8950,7 @@
         <v>0</v>
       </c>
       <c r="J127">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K127">
         <v>0</v>
@@ -8997,7 +8997,7 @@
         <v>0</v>
       </c>
       <c r="J128">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K128">
         <v>0</v>
@@ -9044,7 +9044,7 @@
         <v>0</v>
       </c>
       <c r="J129">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K129">
         <v>0</v>
@@ -9091,7 +9091,7 @@
         <v>0</v>
       </c>
       <c r="J130">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K130">
         <v>0</v>
@@ -9138,7 +9138,7 @@
         <v>0</v>
       </c>
       <c r="J131">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K131">
         <v>0</v>
@@ -9185,7 +9185,7 @@
         <v>0</v>
       </c>
       <c r="J132">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K132">
         <v>0</v>
@@ -9382,7 +9382,7 @@
         <v>0</v>
       </c>
       <c r="J136">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K136">
         <v>0</v>
@@ -9429,7 +9429,7 @@
         <v>0</v>
       </c>
       <c r="J137">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K137">
         <v>0</v>
@@ -9476,7 +9476,7 @@
         <v>0</v>
       </c>
       <c r="J138">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K138">
         <v>0</v>
@@ -9523,7 +9523,7 @@
         <v>0</v>
       </c>
       <c r="J139">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K139">
         <v>0</v>
@@ -9570,7 +9570,7 @@
         <v>0</v>
       </c>
       <c r="J140">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K140">
         <v>0</v>
@@ -9617,7 +9617,7 @@
         <v>0</v>
       </c>
       <c r="J141">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K141">
         <v>0</v>
@@ -9664,7 +9664,7 @@
         <v>0</v>
       </c>
       <c r="J142">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K142">
         <v>0</v>
@@ -9711,7 +9711,7 @@
         <v>0</v>
       </c>
       <c r="J143">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K143">
         <v>0</v>
@@ -9758,7 +9758,7 @@
         <v>0</v>
       </c>
       <c r="J144">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K144">
         <v>0</v>
@@ -9805,7 +9805,7 @@
         <v>0</v>
       </c>
       <c r="J145">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K145">
         <v>0</v>
@@ -9902,7 +9902,7 @@
         <v>0</v>
       </c>
       <c r="J147">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K147">
         <v>0</v>
@@ -10043,7 +10043,7 @@
         <v>0</v>
       </c>
       <c r="J150">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K150">
         <v>0</v>
@@ -10090,7 +10090,7 @@
         <v>0</v>
       </c>
       <c r="J151">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K151">
         <v>0</v>
@@ -10137,7 +10137,7 @@
         <v>0</v>
       </c>
       <c r="J152">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K152">
         <v>0</v>
@@ -10184,7 +10184,7 @@
         <v>0</v>
       </c>
       <c r="J153">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K153">
         <v>0</v>
@@ -10275,7 +10275,7 @@
         <v>0</v>
       </c>
       <c r="J155">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K155">
         <v>0</v>
@@ -10322,7 +10322,7 @@
         <v>0</v>
       </c>
       <c r="J156">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K156">
         <v>0</v>
@@ -10369,7 +10369,7 @@
         <v>0</v>
       </c>
       <c r="J157">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K157">
         <v>0</v>
@@ -10416,7 +10416,7 @@
         <v>0</v>
       </c>
       <c r="J158">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K158">
         <v>0</v>
@@ -10463,7 +10463,7 @@
         <v>0</v>
       </c>
       <c r="J159">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K159">
         <v>0</v>
@@ -10510,7 +10510,7 @@
         <v>0</v>
       </c>
       <c r="J160">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K160">
         <v>0</v>
@@ -10557,7 +10557,7 @@
         <v>0</v>
       </c>
       <c r="J161">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K161">
         <v>0</v>
@@ -10604,7 +10604,7 @@
         <v>0</v>
       </c>
       <c r="J162">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K162">
         <v>0</v>
@@ -10751,7 +10751,7 @@
         <v>0</v>
       </c>
       <c r="J165">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K165">
         <v>0</v>
@@ -10798,7 +10798,7 @@
         <v>0</v>
       </c>
       <c r="J166">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K166">
         <v>0</v>
@@ -10845,7 +10845,7 @@
         <v>0</v>
       </c>
       <c r="J167">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K167">
         <v>0</v>
@@ -10936,7 +10936,7 @@
         <v>0</v>
       </c>
       <c r="J169">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K169">
         <v>0</v>
@@ -10983,7 +10983,7 @@
         <v>0</v>
       </c>
       <c r="J170">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K170">
         <v>0</v>
@@ -11030,7 +11030,7 @@
         <v>0</v>
       </c>
       <c r="J171">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K171">
         <v>0</v>
@@ -11077,7 +11077,7 @@
         <v>0</v>
       </c>
       <c r="J172">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K172">
         <v>0</v>
@@ -11124,7 +11124,7 @@
         <v>0</v>
       </c>
       <c r="J173">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K173">
         <v>0</v>
@@ -11171,7 +11171,7 @@
         <v>0</v>
       </c>
       <c r="J174">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K174">
         <v>0</v>
@@ -11268,7 +11268,7 @@
         <v>0</v>
       </c>
       <c r="J176">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K176">
         <v>0</v>
@@ -11315,7 +11315,7 @@
         <v>0</v>
       </c>
       <c r="J177">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K177">
         <v>0</v>
@@ -11362,7 +11362,7 @@
         <v>0</v>
       </c>
       <c r="J178">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K178">
         <v>0</v>
@@ -11509,7 +11509,7 @@
         <v>0</v>
       </c>
       <c r="J181">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K181">
         <v>0</v>
@@ -11650,7 +11650,7 @@
         <v>0</v>
       </c>
       <c r="J184">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K184">
         <v>0</v>
@@ -11747,7 +11747,7 @@
         <v>0</v>
       </c>
       <c r="J186">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K186">
         <v>0</v>
@@ -11888,7 +11888,7 @@
         <v>0</v>
       </c>
       <c r="J189">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K189">
         <v>0</v>
@@ -11935,7 +11935,7 @@
         <v>0</v>
       </c>
       <c r="J190">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K190">
         <v>0</v>
@@ -11982,7 +11982,7 @@
         <v>0</v>
       </c>
       <c r="J191">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K191">
         <v>0</v>
@@ -12029,7 +12029,7 @@
         <v>0</v>
       </c>
       <c r="J192">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K192">
         <v>0</v>
@@ -12126,7 +12126,7 @@
         <v>0</v>
       </c>
       <c r="J194">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K194">
         <v>0</v>
@@ -12173,7 +12173,7 @@
         <v>0</v>
       </c>
       <c r="J195">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K195">
         <v>0</v>
@@ -12264,7 +12264,7 @@
         <v>0</v>
       </c>
       <c r="J197">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K197">
         <v>0</v>
@@ -12311,7 +12311,7 @@
         <v>0</v>
       </c>
       <c r="J198">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K198">
         <v>0</v>
@@ -12358,7 +12358,7 @@
         <v>0</v>
       </c>
       <c r="J199">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K199">
         <v>0</v>
@@ -12405,7 +12405,7 @@
         <v>0</v>
       </c>
       <c r="J200">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K200">
         <v>0</v>
@@ -12452,7 +12452,7 @@
         <v>0</v>
       </c>
       <c r="J201">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K201">
         <v>0</v>
@@ -12499,7 +12499,7 @@
         <v>0</v>
       </c>
       <c r="J202">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K202">
         <v>0</v>
@@ -12546,7 +12546,7 @@
         <v>0</v>
       </c>
       <c r="J203">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K203">
         <v>0</v>
@@ -12637,7 +12637,7 @@
         <v>0</v>
       </c>
       <c r="J205">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K205">
         <v>0</v>
@@ -12734,7 +12734,7 @@
         <v>0</v>
       </c>
       <c r="J207">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K207">
         <v>0</v>
@@ -12825,7 +12825,7 @@
         <v>0</v>
       </c>
       <c r="J209">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K209">
         <v>0</v>
@@ -12922,7 +12922,7 @@
         <v>0</v>
       </c>
       <c r="J211">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K211">
         <v>0</v>
@@ -12969,7 +12969,7 @@
         <v>0</v>
       </c>
       <c r="J212">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K212">
         <v>0</v>
@@ -13016,7 +13016,7 @@
         <v>0</v>
       </c>
       <c r="J213">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K213">
         <v>0</v>
@@ -13063,7 +13063,7 @@
         <v>0</v>
       </c>
       <c r="J214">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K214">
         <v>0</v>
@@ -13110,7 +13110,7 @@
         <v>0</v>
       </c>
       <c r="J215">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K215">
         <v>0</v>
@@ -13157,7 +13157,7 @@
         <v>0</v>
       </c>
       <c r="J216">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K216">
         <v>0</v>
@@ -13204,7 +13204,7 @@
         <v>0</v>
       </c>
       <c r="J217">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K217">
         <v>0</v>
@@ -13251,7 +13251,7 @@
         <v>0</v>
       </c>
       <c r="J218">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K218">
         <v>0</v>
@@ -13298,7 +13298,7 @@
         <v>0</v>
       </c>
       <c r="J219">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K219">
         <v>0</v>
@@ -13395,7 +13395,7 @@
         <v>0</v>
       </c>
       <c r="J221">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K221">
         <v>0</v>
@@ -13442,7 +13442,7 @@
         <v>0</v>
       </c>
       <c r="J222">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K222">
         <v>0</v>
@@ -13489,7 +13489,7 @@
         <v>0</v>
       </c>
       <c r="J223">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K223">
         <v>0</v>
@@ -13680,7 +13680,7 @@
         <v>0</v>
       </c>
       <c r="J227">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K227">
         <v>0</v>
@@ -13777,7 +13777,7 @@
         <v>0</v>
       </c>
       <c r="J229">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K229">
         <v>0</v>
@@ -13918,7 +13918,7 @@
         <v>0</v>
       </c>
       <c r="J232">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K232">
         <v>0</v>
@@ -13965,7 +13965,7 @@
         <v>0</v>
       </c>
       <c r="J233">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K233">
         <v>0</v>
@@ -14012,7 +14012,7 @@
         <v>0</v>
       </c>
       <c r="J234">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K234">
         <v>0</v>
@@ -14059,7 +14059,7 @@
         <v>0</v>
       </c>
       <c r="J235">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K235">
         <v>0</v>
@@ -14156,7 +14156,7 @@
         <v>0</v>
       </c>
       <c r="J237">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K237">
         <v>0</v>
@@ -14203,7 +14203,7 @@
         <v>0</v>
       </c>
       <c r="J238">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K238">
         <v>0</v>
@@ -14250,7 +14250,7 @@
         <v>0</v>
       </c>
       <c r="J239">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K239">
         <v>0</v>
@@ -14297,7 +14297,7 @@
         <v>0</v>
       </c>
       <c r="J240">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K240">
         <v>0</v>
@@ -14344,7 +14344,7 @@
         <v>0</v>
       </c>
       <c r="J241">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K241">
         <v>0</v>
@@ -14391,7 +14391,7 @@
         <v>0</v>
       </c>
       <c r="J242">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K242">
         <v>0</v>
@@ -14482,7 +14482,7 @@
         <v>0</v>
       </c>
       <c r="J244">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K244">
         <v>0</v>
@@ -14529,7 +14529,7 @@
         <v>0</v>
       </c>
       <c r="J245">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K245">
         <v>0</v>
@@ -14576,7 +14576,7 @@
         <v>0</v>
       </c>
       <c r="J246">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K246">
         <v>0</v>
@@ -14623,7 +14623,7 @@
         <v>0</v>
       </c>
       <c r="J247">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K247">
         <v>0</v>
@@ -14670,7 +14670,7 @@
         <v>0</v>
       </c>
       <c r="J248">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K248">
         <v>0</v>
@@ -14767,7 +14767,7 @@
         <v>0</v>
       </c>
       <c r="J250">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K250">
         <v>0</v>
@@ -14814,7 +14814,7 @@
         <v>0</v>
       </c>
       <c r="J251">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K251">
         <v>0</v>
@@ -14861,7 +14861,7 @@
         <v>0</v>
       </c>
       <c r="J252">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K252">
         <v>0</v>
@@ -14908,7 +14908,7 @@
         <v>0</v>
       </c>
       <c r="J253">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K253">
         <v>0</v>
@@ -14999,7 +14999,7 @@
         <v>0</v>
       </c>
       <c r="J255">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K255">
         <v>0</v>
@@ -15046,7 +15046,7 @@
         <v>0</v>
       </c>
       <c r="J256">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K256">
         <v>0</v>
@@ -15093,7 +15093,7 @@
         <v>0</v>
       </c>
       <c r="J257">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K257">
         <v>0</v>
@@ -15284,7 +15284,7 @@
         <v>0</v>
       </c>
       <c r="J261">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K261">
         <v>0</v>
@@ -15331,7 +15331,7 @@
         <v>0</v>
       </c>
       <c r="J262">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K262">
         <v>0</v>
@@ -15378,7 +15378,7 @@
         <v>0</v>
       </c>
       <c r="J263">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K263">
         <v>0</v>
@@ -15469,7 +15469,7 @@
         <v>0</v>
       </c>
       <c r="J265">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K265">
         <v>0</v>
@@ -15716,7 +15716,7 @@
         <v>0</v>
       </c>
       <c r="J270">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K270">
         <v>0</v>
@@ -15763,7 +15763,7 @@
         <v>0</v>
       </c>
       <c r="J271">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K271">
         <v>0</v>
@@ -15810,7 +15810,7 @@
         <v>0</v>
       </c>
       <c r="J272">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K272">
         <v>0</v>
@@ -15857,7 +15857,7 @@
         <v>0</v>
       </c>
       <c r="J273">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K273">
         <v>0</v>
@@ -15904,7 +15904,7 @@
         <v>0</v>
       </c>
       <c r="J274">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K274">
         <v>0</v>
@@ -15951,7 +15951,7 @@
         <v>0</v>
       </c>
       <c r="J275">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K275">
         <v>0</v>
@@ -16042,7 +16042,7 @@
         <v>0</v>
       </c>
       <c r="J277">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K277">
         <v>0</v>
@@ -16139,7 +16139,7 @@
         <v>0</v>
       </c>
       <c r="J279">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K279">
         <v>0</v>
@@ -16186,7 +16186,7 @@
         <v>0</v>
       </c>
       <c r="J280">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K280">
         <v>0</v>
@@ -16283,7 +16283,7 @@
         <v>0</v>
       </c>
       <c r="J282">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K282">
         <v>0</v>
@@ -16380,7 +16380,7 @@
         <v>0</v>
       </c>
       <c r="J284">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K284">
         <v>0</v>
@@ -16477,7 +16477,7 @@
         <v>0</v>
       </c>
       <c r="J286">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K286">
         <v>0</v>
@@ -16574,7 +16574,7 @@
         <v>0</v>
       </c>
       <c r="J288">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K288">
         <v>0</v>
@@ -16621,7 +16621,7 @@
         <v>0</v>
       </c>
       <c r="J289">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K289">
         <v>0</v>
@@ -16668,7 +16668,7 @@
         <v>0</v>
       </c>
       <c r="J290">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K290">
         <v>0</v>
@@ -16715,7 +16715,7 @@
         <v>0</v>
       </c>
       <c r="J291">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K291">
         <v>0</v>
@@ -16762,7 +16762,7 @@
         <v>0</v>
       </c>
       <c r="J292">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K292">
         <v>0</v>
@@ -16859,7 +16859,7 @@
         <v>0</v>
       </c>
       <c r="J294">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K294">
         <v>0</v>
@@ -16956,7 +16956,7 @@
         <v>0</v>
       </c>
       <c r="J296">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K296">
         <v>0</v>
@@ -17053,7 +17053,7 @@
         <v>0</v>
       </c>
       <c r="J298">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K298">
         <v>0</v>
@@ -17100,7 +17100,7 @@
         <v>0</v>
       </c>
       <c r="J299">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K299">
         <v>0</v>
@@ -17147,7 +17147,7 @@
         <v>0</v>
       </c>
       <c r="J300">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K300">
         <v>0</v>
@@ -17294,7 +17294,7 @@
         <v>0</v>
       </c>
       <c r="J303">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K303">
         <v>0</v>
@@ -17341,7 +17341,7 @@
         <v>0</v>
       </c>
       <c r="J304">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K304">
         <v>0</v>
@@ -17388,7 +17388,7 @@
         <v>0</v>
       </c>
       <c r="J305">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K305">
         <v>0</v>
@@ -17435,7 +17435,7 @@
         <v>0</v>
       </c>
       <c r="J306">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K306">
         <v>0</v>
@@ -17526,7 +17526,7 @@
         <v>0</v>
       </c>
       <c r="J308">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K308">
         <v>0</v>
@@ -17623,7 +17623,7 @@
         <v>0</v>
       </c>
       <c r="J310">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K310">
         <v>0</v>
@@ -17670,7 +17670,7 @@
         <v>0</v>
       </c>
       <c r="J311">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K311">
         <v>0</v>
@@ -17717,7 +17717,7 @@
         <v>0</v>
       </c>
       <c r="J312">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K312">
         <v>0</v>
@@ -17955,7 +17955,7 @@
         <v>0</v>
       </c>
       <c r="J317">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K317">
         <v>0</v>
@@ -18052,7 +18052,7 @@
         <v>0</v>
       </c>
       <c r="J319">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K319">
         <v>0</v>
@@ -18149,7 +18149,7 @@
         <v>0</v>
       </c>
       <c r="J321">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K321">
         <v>0</v>
@@ -18196,7 +18196,7 @@
         <v>0</v>
       </c>
       <c r="J322">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K322">
         <v>0</v>
@@ -18287,7 +18287,7 @@
         <v>0</v>
       </c>
       <c r="J324">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K324">
         <v>0</v>
@@ -18334,7 +18334,7 @@
         <v>0</v>
       </c>
       <c r="J325">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K325">
         <v>0</v>
@@ -18381,7 +18381,7 @@
         <v>0</v>
       </c>
       <c r="J326">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K326">
         <v>0</v>
@@ -18472,7 +18472,7 @@
         <v>0</v>
       </c>
       <c r="J328">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K328">
         <v>0</v>
@@ -18519,7 +18519,7 @@
         <v>0</v>
       </c>
       <c r="J329">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K329">
         <v>0</v>
@@ -18566,7 +18566,7 @@
         <v>0</v>
       </c>
       <c r="J330">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K330">
         <v>0</v>
@@ -18707,7 +18707,7 @@
         <v>0</v>
       </c>
       <c r="J333">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K333">
         <v>0</v>
@@ -18804,7 +18804,7 @@
         <v>0</v>
       </c>
       <c r="J335">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K335">
         <v>0</v>
@@ -18951,7 +18951,7 @@
         <v>0</v>
       </c>
       <c r="J338">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K338">
         <v>0</v>
@@ -19048,7 +19048,7 @@
         <v>0</v>
       </c>
       <c r="J340">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K340">
         <v>0</v>
@@ -19095,7 +19095,7 @@
         <v>0</v>
       </c>
       <c r="J341">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K341">
         <v>0</v>
@@ -19142,7 +19142,7 @@
         <v>0</v>
       </c>
       <c r="J342">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K342">
         <v>0</v>
@@ -19189,7 +19189,7 @@
         <v>0</v>
       </c>
       <c r="J343">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K343">
         <v>0</v>
@@ -19236,7 +19236,7 @@
         <v>0</v>
       </c>
       <c r="J344">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K344">
         <v>0</v>
@@ -19483,7 +19483,7 @@
         <v>0</v>
       </c>
       <c r="J349">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K349">
         <v>0</v>
@@ -19530,7 +19530,7 @@
         <v>0</v>
       </c>
       <c r="J350">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K350">
         <v>0</v>
@@ -19577,7 +19577,7 @@
         <v>0</v>
       </c>
       <c r="J351">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K351">
         <v>0</v>
@@ -19674,7 +19674,7 @@
         <v>0</v>
       </c>
       <c r="J353">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K353">
         <v>0</v>
@@ -19915,7 +19915,7 @@
         <v>0</v>
       </c>
       <c r="J358">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K358">
         <v>0</v>
@@ -19962,7 +19962,7 @@
         <v>0</v>
       </c>
       <c r="J359">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K359">
         <v>0</v>
@@ -20009,7 +20009,7 @@
         <v>0</v>
       </c>
       <c r="J360">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K360">
         <v>0</v>
@@ -20056,7 +20056,7 @@
         <v>0</v>
       </c>
       <c r="J361">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K361">
         <v>0</v>
@@ -20153,7 +20153,7 @@
         <v>0</v>
       </c>
       <c r="J363">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K363">
         <v>0</v>
@@ -20200,7 +20200,7 @@
         <v>0</v>
       </c>
       <c r="J364">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K364">
         <v>0</v>
@@ -20247,7 +20247,7 @@
         <v>0</v>
       </c>
       <c r="J365">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K365">
         <v>0</v>
@@ -20438,7 +20438,7 @@
         <v>0</v>
       </c>
       <c r="J369">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K369">
         <v>0</v>
@@ -20485,7 +20485,7 @@
         <v>0</v>
       </c>
       <c r="J370">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K370">
         <v>0</v>
@@ -20582,7 +20582,7 @@
         <v>0</v>
       </c>
       <c r="J372">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K372">
         <v>0</v>
@@ -20629,7 +20629,7 @@
         <v>0</v>
       </c>
       <c r="J373">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K373">
         <v>0</v>
@@ -20676,7 +20676,7 @@
         <v>0</v>
       </c>
       <c r="J374">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K374">
         <v>0</v>
@@ -20723,7 +20723,7 @@
         <v>0</v>
       </c>
       <c r="J375">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K375">
         <v>0</v>
@@ -20770,7 +20770,7 @@
         <v>0</v>
       </c>
       <c r="J376">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K376">
         <v>0</v>
@@ -20817,7 +20817,7 @@
         <v>0</v>
       </c>
       <c r="J377">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K377">
         <v>0</v>
@@ -20964,7 +20964,7 @@
         <v>0</v>
       </c>
       <c r="J380">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K380">
         <v>0</v>
@@ -21111,7 +21111,7 @@
         <v>0</v>
       </c>
       <c r="J383">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K383">
         <v>0</v>
@@ -21158,7 +21158,7 @@
         <v>0</v>
       </c>
       <c r="J384">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K384">
         <v>0</v>
@@ -21205,7 +21205,7 @@
         <v>0</v>
       </c>
       <c r="J385">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K385">
         <v>0</v>
@@ -21252,7 +21252,7 @@
         <v>0</v>
       </c>
       <c r="J386">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K386">
         <v>0</v>
@@ -21299,7 +21299,7 @@
         <v>0</v>
       </c>
       <c r="J387">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K387">
         <v>0</v>
@@ -21346,7 +21346,7 @@
         <v>0</v>
       </c>
       <c r="J388">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K388">
         <v>0</v>
@@ -21393,7 +21393,7 @@
         <v>0</v>
       </c>
       <c r="J389">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K389">
         <v>0</v>
@@ -21540,7 +21540,7 @@
         <v>0</v>
       </c>
       <c r="J392">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K392">
         <v>0</v>
@@ -21587,7 +21587,7 @@
         <v>0</v>
       </c>
       <c r="J393">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K393">
         <v>0</v>
@@ -21678,7 +21678,7 @@
         <v>0</v>
       </c>
       <c r="J395">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K395">
         <v>0</v>
@@ -21725,7 +21725,7 @@
         <v>0</v>
       </c>
       <c r="J396">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K396">
         <v>0</v>
@@ -21772,7 +21772,7 @@
         <v>0</v>
       </c>
       <c r="J397">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K397">
         <v>0</v>
@@ -21869,7 +21869,7 @@
         <v>0</v>
       </c>
       <c r="J399">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K399">
         <v>0</v>
@@ -21916,7 +21916,7 @@
         <v>0</v>
       </c>
       <c r="J400">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K400">
         <v>0</v>
@@ -21963,7 +21963,7 @@
         <v>0</v>
       </c>
       <c r="J401">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K401">
         <v>0</v>
@@ -22060,7 +22060,7 @@
         <v>0</v>
       </c>
       <c r="J403">
-        <v>1587083823.630226</v>
+        <v>1587089010.639998</v>
       </c>
       <c r="K403">
         <v>0</v>

</xml_diff>